<commit_message>
updates for first dry run ready
</commit_message>
<xml_diff>
--- a/Resources/MoviesToWatch.xlsx
+++ b/Resources/MoviesToWatch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\acw_work\FunctionAppStarter\DataProcessingFunctions\ParseExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF612FB-CFD1-4CF3-8746-67DD20E63D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80DAF85-33FE-44FA-ABEC-C691A5811F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28875" yWindow="2685" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Title</t>
   </si>
@@ -73,6 +70,27 @@
   </si>
   <si>
     <t>Dungeons &amp; Dragons: Honor Among Thieves</t>
+  </si>
+  <si>
+    <t>MovieId</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>a5521c81-8a9e-4ac5-8031-52008277c4ec</t>
+  </si>
+  <si>
+    <t>62ae2134-1ad3-4496-af69-e86318abb836</t>
+  </si>
+  <si>
+    <t>b21ea323-8d40-42c7-91f3-213e5dbfef55</t>
+  </si>
+  <si>
+    <t>ae53c082-b231-4dab-9647-900d066eeed8</t>
+  </si>
+  <si>
+    <t>1a6b4927-ac51-4453-8d82-5a7227511e09</t>
   </si>
 </sst>
 </file>
@@ -390,118 +408,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>1999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3">
-        <v>1998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E6" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6">
+      <c r="F6">
         <v>2023</v>
       </c>
     </row>

</xml_diff>